<commit_message>
add instructions and and sound for GOS
</commit_message>
<xml_diff>
--- a/LevelDesign_excel/Level2.xlsx
+++ b/LevelDesign_excel/Level2.xlsx
@@ -767,7 +767,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -781,7 +781,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1105,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" topLeftCell="K24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF31" sqref="AF31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6341,10 +6341,10 @@
         <v>9</v>
       </c>
       <c r="AD34" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="22">
         <v>9</v>
-      </c>
-      <c r="AE34" s="22">
-        <v>0</v>
       </c>
       <c r="AF34" s="22">
         <v>9</v>
@@ -6490,10 +6490,10 @@
         <v>1</v>
       </c>
       <c r="AC35" s="20">
+        <v>14</v>
+      </c>
+      <c r="AD35" s="22">
         <v>9</v>
-      </c>
-      <c r="AD35" s="22">
-        <v>14</v>
       </c>
       <c r="AE35" s="22">
         <v>9</v>
@@ -9018,13 +9018,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AX51">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>30</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>31</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>